<commit_message>
New changes - 16/7
5/18
</commit_message>
<xml_diff>
--- a/utilities/ALM_Data.xlsx
+++ b/utilities/ALM_Data.xlsx
@@ -8,19 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ProjectTree_QA\Selenium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54298F04-4BB2-40EB-AD17-B5EDA6908444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76CAC2FD-6AC3-48A1-B578-1FD1121CCBD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Add Test Case" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
+  <si>
+    <t>MTC</t>
+  </si>
   <si>
     <t>username</t>
   </si>
@@ -28,9 +32,15 @@
     <t>password</t>
   </si>
   <si>
+    <t>Expected Text</t>
+  </si>
+  <si>
     <t>Remarks</t>
   </si>
   <si>
+    <t>MTC_001</t>
+  </si>
+  <si>
     <t>hiteshpatel1487</t>
   </si>
   <si>
@@ -43,6 +53,9 @@
     <t>Valid login</t>
   </si>
   <si>
+    <t>MTC_002</t>
+  </si>
+  <si>
     <t>invaliduser</t>
   </si>
   <si>
@@ -55,44 +68,56 @@
     <t>Invalid login</t>
   </si>
   <si>
+    <t>MTC_003</t>
+  </si>
+  <si>
     <t>Username or Email is required</t>
   </si>
   <si>
+    <t>MTC_004</t>
+  </si>
+  <si>
     <t>Password is required</t>
   </si>
   <si>
+    <t>MTC_005</t>
+  </si>
+  <si>
+    <t>MTC_006</t>
+  </si>
+  <si>
     <t>hiteshpatel</t>
   </si>
   <si>
-    <t>Expected Text</t>
-  </si>
-  <si>
-    <t>MTC</t>
-  </si>
-  <si>
-    <t>MTC_001</t>
-  </si>
-  <si>
-    <t>MTC_002</t>
-  </si>
-  <si>
-    <t>MTC_003</t>
-  </si>
-  <si>
-    <t>MTC_004</t>
-  </si>
-  <si>
-    <t>MTC_005</t>
-  </si>
-  <si>
-    <t>MTC_006</t>
+    <t>Test Case Name</t>
+  </si>
+  <si>
+    <t>Step</t>
+  </si>
+  <si>
+    <t>Automation</t>
+  </si>
+  <si>
+    <t>Test Case Title</t>
+  </si>
+  <si>
+    <t>MTC_008</t>
+  </si>
+  <si>
+    <t>MTC_009</t>
+  </si>
+  <si>
+    <t>MTC_010</t>
+  </si>
+  <si>
+    <t>MTC_011</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,17 +129,6 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="Var(--jp-code-font-family)"/>
     </font>
   </fonts>
   <fills count="2">
@@ -157,8 +171,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -464,128 +478,187 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C29" sqref="C28:C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B24AF94F-FFD4-4040-81F0-5728AF98C648}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>16</v>
+        <v>23</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" t="s">
-        <v>10</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>